<commit_message>
adaptation to new scales
</commit_message>
<xml_diff>
--- a/psychometric_scale/stuff/GSE.xlsx
+++ b/psychometric_scale/stuff/GSE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabienvinckier/Desktop/home/projects/git/Misc/psychometric_scale/stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Desktop/psychometric_scale/stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1C664F64-847F-D543-8A52-CDACF8F02648}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1160" windowWidth="27200" windowHeight="16540" activeTab="1"/>
+    <workbookView xWindow="1200" yWindow="1160" windowWidth="27200" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +34,6 @@
     <t>Comment pensez-vous que le traitement par ECT va affecter (ou a affecté) votre mémoire ?</t>
   </si>
   <si>
-    <t xml:space="preserve">1 \n\n Effet extremement négatif </t>
-  </si>
-  <si>
     <t xml:space="preserve">2 \n\n  </t>
   </si>
   <si>
@@ -52,12 +50,15 @@
   </si>
   <si>
     <t>7 \n\n Effet extrêmement positif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 \n\n Effet extrêmement négatif </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,7 +404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -428,36 +429,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>